<commit_message>
created convictions table to prep for appendix 3
</commit_message>
<xml_diff>
--- a/sourcefiles/convictionstable.xlsx
+++ b/sourcefiles/convictionstable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendan/Documents/epubs/TRC/truth-and-reconciliation-commission-of-canada_honouring-the-truth-reconciling-for-the-future/sourcefiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A976605B-C970-9C44-B32B-1E0684E30102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D173A7D-EDC6-2D4E-9BF4-DE0CD53B8926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14780" yWindow="2800" windowWidth="31160" windowHeight="21140" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D48" sqref="A1:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>